<commit_message>
created some crud methods of employees
</commit_message>
<xml_diff>
--- a/Controle.xlsx
+++ b/Controle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jardel\Desktop\Estudos Spring MVC\BarberSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D94BC72-C6A5-416B-BA68-B97FF6C1FF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62015E8-69AE-45EE-891D-9F868743C4E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Produção</t>
   </si>
@@ -70,6 +70,32 @@
   </si>
   <si>
     <t>Tela de Catálogo dos produtos cadastrados</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Primeiro vamos focar no básico (CRUD normal). Depois, quando você implementar o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Spring Security</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, aí a gente bloqueia o acesso via roles</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -414,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,6 +538,11 @@
       </c>
       <c r="B14" s="1"/>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>